<commit_message>
Regenerate database with new stat order: PTS/REB/AST/STL/BLK
</commit_message>
<xml_diff>
--- a/CurrentSeason_UniqornGames_Master.xlsx
+++ b/CurrentSeason_UniqornGames_Master.xlsx
@@ -523,10 +523,10 @@
         <v>6</v>
       </c>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -563,10 +563,10 @@
         <v>2</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -603,10 +603,10 @@
         <v>17</v>
       </c>
       <c r="I4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -643,10 +643,10 @@
         <v>6</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -763,10 +763,10 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -803,10 +803,10 @@
         <v>5</v>
       </c>
       <c r="I9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -843,10 +843,10 @@
         <v>13</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -883,10 +883,10 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -923,10 +923,10 @@
         <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J12" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -963,10 +963,10 @@
         <v>11</v>
       </c>
       <c r="I13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -1003,10 +1003,10 @@
         <v>15</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1043,10 +1043,10 @@
         <v>9</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1083,10 +1083,10 @@
         <v>9</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1123,10 +1123,10 @@
         <v>2</v>
       </c>
       <c r="I17" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" t="n">
         <v>5</v>
-      </c>
-      <c r="J17" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1163,10 +1163,10 @@
         <v>9</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1203,10 +1203,10 @@
         <v>5</v>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1243,10 +1243,10 @@
         <v>1</v>
       </c>
       <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
         <v>5</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1283,10 +1283,10 @@
         <v>22</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1323,10 +1323,10 @@
         <v>8</v>
       </c>
       <c r="I22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1363,10 +1363,10 @@
         <v>2</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1403,10 +1403,10 @@
         <v>12</v>
       </c>
       <c r="I24" t="n">
+        <v>4</v>
+      </c>
+      <c r="J24" t="n">
         <v>3</v>
-      </c>
-      <c r="J24" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -1443,10 +1443,10 @@
         <v>5</v>
       </c>
       <c r="I25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1483,10 +1483,10 @@
         <v>12</v>
       </c>
       <c r="I26" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J26" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -1523,10 +1523,10 @@
         <v>5</v>
       </c>
       <c r="I27" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
@@ -1563,10 +1563,10 @@
         <v>13</v>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1603,10 +1603,10 @@
         <v>3</v>
       </c>
       <c r="I29" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
@@ -1683,10 +1683,10 @@
         <v>9</v>
       </c>
       <c r="I31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1723,10 +1723,10 @@
         <v>2</v>
       </c>
       <c r="I32" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J32" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -1763,10 +1763,10 @@
         <v>2</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1803,10 +1803,10 @@
         <v>1</v>
       </c>
       <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
         <v>6</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1843,10 +1843,10 @@
         <v>9</v>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J35" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1883,10 +1883,10 @@
         <v>6</v>
       </c>
       <c r="I36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1923,10 +1923,10 @@
         <v>4</v>
       </c>
       <c r="I37" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
@@ -1963,10 +1963,10 @@
         <v>5</v>
       </c>
       <c r="I38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J38" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -2003,10 +2003,10 @@
         <v>3</v>
       </c>
       <c r="I39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J39" t="n">
         <v>5</v>
-      </c>
-      <c r="J39" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -2043,10 +2043,10 @@
         <v>5</v>
       </c>
       <c r="I40" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J40" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -2083,10 +2083,10 @@
         <v>2</v>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J42" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -2163,10 +2163,10 @@
         <v>3</v>
       </c>
       <c r="I43" t="n">
+        <v>2</v>
+      </c>
+      <c r="J43" t="n">
         <v>6</v>
-      </c>
-      <c r="J43" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -2203,10 +2203,10 @@
         <v>3</v>
       </c>
       <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
         <v>5</v>
-      </c>
-      <c r="J44" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -2283,10 +2283,10 @@
         <v>3</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J46" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2323,10 +2323,10 @@
         <v>0</v>
       </c>
       <c r="I47" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -2363,10 +2363,10 @@
         <v>8</v>
       </c>
       <c r="I48" t="n">
+        <v>1</v>
+      </c>
+      <c r="J48" t="n">
         <v>3</v>
-      </c>
-      <c r="J48" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2403,10 +2403,10 @@
         <v>7</v>
       </c>
       <c r="I49" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -2443,10 +2443,10 @@
         <v>4</v>
       </c>
       <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
         <v>6</v>
-      </c>
-      <c r="J50" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2483,10 +2483,10 @@
         <v>2</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J51" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2523,10 +2523,10 @@
         <v>3</v>
       </c>
       <c r="I52" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
@@ -2563,10 +2563,10 @@
         <v>1</v>
       </c>
       <c r="I53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J53" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
@@ -2603,10 +2603,10 @@
         <v>3</v>
       </c>
       <c r="I54" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J54" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55">
@@ -2643,10 +2643,10 @@
         <v>12</v>
       </c>
       <c r="I55" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" t="n">
         <v>3</v>
-      </c>
-      <c r="J55" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2683,10 +2683,10 @@
         <v>9</v>
       </c>
       <c r="I56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -2723,10 +2723,10 @@
         <v>8</v>
       </c>
       <c r="I57" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J57" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -2763,10 +2763,10 @@
         <v>14</v>
       </c>
       <c r="I58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -2803,10 +2803,10 @@
         <v>6</v>
       </c>
       <c r="I59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2923,10 +2923,10 @@
         <v>9</v>
       </c>
       <c r="I62" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J62" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -2963,10 +2963,10 @@
         <v>6</v>
       </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J63" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -3043,10 +3043,10 @@
         <v>4</v>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J65" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -3083,10 +3083,10 @@
         <v>0</v>
       </c>
       <c r="I66" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J66" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -3123,10 +3123,10 @@
         <v>13</v>
       </c>
       <c r="I67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -3163,10 +3163,10 @@
         <v>5</v>
       </c>
       <c r="I68" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J68" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
@@ -3203,10 +3203,10 @@
         <v>6</v>
       </c>
       <c r="I69" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J69" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -3243,10 +3243,10 @@
         <v>1</v>
       </c>
       <c r="I70" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J70" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -3283,10 +3283,10 @@
         <v>1</v>
       </c>
       <c r="I71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -3363,10 +3363,10 @@
         <v>6</v>
       </c>
       <c r="I73" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J73" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -3403,10 +3403,10 @@
         <v>1</v>
       </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J74" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -3443,10 +3443,10 @@
         <v>10</v>
       </c>
       <c r="I75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -3483,10 +3483,10 @@
         <v>12</v>
       </c>
       <c r="I76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -3523,10 +3523,10 @@
         <v>10</v>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J77" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -3563,10 +3563,10 @@
         <v>15</v>
       </c>
       <c r="I78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -3603,10 +3603,10 @@
         <v>6</v>
       </c>
       <c r="I79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J79" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -3643,10 +3643,10 @@
         <v>2</v>
       </c>
       <c r="I80" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J80" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -3723,10 +3723,10 @@
         <v>9</v>
       </c>
       <c r="I82" t="n">
+        <v>2</v>
+      </c>
+      <c r="J82" t="n">
         <v>3</v>
-      </c>
-      <c r="J82" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -3763,10 +3763,10 @@
         <v>13</v>
       </c>
       <c r="I83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -3803,10 +3803,10 @@
         <v>6</v>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -3843,10 +3843,10 @@
         <v>10</v>
       </c>
       <c r="I85" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J85" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
@@ -3883,10 +3883,10 @@
         <v>3</v>
       </c>
       <c r="I86" t="n">
+        <v>4</v>
+      </c>
+      <c r="J86" t="n">
         <v>3</v>
-      </c>
-      <c r="J86" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -3963,10 +3963,10 @@
         <v>8</v>
       </c>
       <c r="I88" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" t="n">
         <v>3</v>
-      </c>
-      <c r="J88" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -4043,10 +4043,10 @@
         <v>3</v>
       </c>
       <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="n">
         <v>5</v>
-      </c>
-      <c r="J90" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -4083,10 +4083,10 @@
         <v>4</v>
       </c>
       <c r="I91" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J91" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92">
@@ -4203,10 +4203,10 @@
         <v>1</v>
       </c>
       <c r="I94" t="n">
+        <v>2</v>
+      </c>
+      <c r="J94" t="n">
         <v>6</v>
-      </c>
-      <c r="J94" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -4243,10 +4243,10 @@
         <v>4</v>
       </c>
       <c r="I95" t="n">
+        <v>2</v>
+      </c>
+      <c r="J95" t="n">
         <v>5</v>
-      </c>
-      <c r="J95" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="96">
@@ -4283,10 +4283,10 @@
         <v>6</v>
       </c>
       <c r="I96" t="n">
+        <v>0</v>
+      </c>
+      <c r="J96" t="n">
         <v>7</v>
-      </c>
-      <c r="J96" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -4363,10 +4363,10 @@
         <v>10</v>
       </c>
       <c r="I98" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J98" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -4403,10 +4403,10 @@
         <v>2</v>
       </c>
       <c r="I99" t="n">
+        <v>5</v>
+      </c>
+      <c r="J99" t="n">
         <v>3</v>
-      </c>
-      <c r="J99" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="100">
@@ -4443,10 +4443,10 @@
         <v>1</v>
       </c>
       <c r="I100" t="n">
+        <v>2</v>
+      </c>
+      <c r="J100" t="n">
         <v>6</v>
-      </c>
-      <c r="J100" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="101">
@@ -4483,10 +4483,10 @@
         <v>5</v>
       </c>
       <c r="I101" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J101" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -4523,10 +4523,10 @@
         <v>1</v>
       </c>
       <c r="I102" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J102" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103">
@@ -4563,10 +4563,10 @@
         <v>9</v>
       </c>
       <c r="I103" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J103" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -4603,10 +4603,10 @@
         <v>1</v>
       </c>
       <c r="I104" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J104" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
@@ -4643,10 +4643,10 @@
         <v>3</v>
       </c>
       <c r="I105" t="n">
+        <v>0</v>
+      </c>
+      <c r="J105" t="n">
         <v>5</v>
-      </c>
-      <c r="J105" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -4723,10 +4723,10 @@
         <v>4</v>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J107" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -4763,10 +4763,10 @@
         <v>0</v>
       </c>
       <c r="I108" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" t="n">
         <v>6</v>
-      </c>
-      <c r="J108" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -4803,10 +4803,10 @@
         <v>15</v>
       </c>
       <c r="I109" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J109" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -4843,10 +4843,10 @@
         <v>14</v>
       </c>
       <c r="I110" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J110" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -4923,10 +4923,10 @@
         <v>10</v>
       </c>
       <c r="I112" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J112" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -4963,10 +4963,10 @@
         <v>2</v>
       </c>
       <c r="I113" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J113" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -5003,10 +5003,10 @@
         <v>2</v>
       </c>
       <c r="I114" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J114" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
@@ -5043,10 +5043,10 @@
         <v>9</v>
       </c>
       <c r="I115" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J115" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -5123,10 +5123,10 @@
         <v>9</v>
       </c>
       <c r="I117" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J117" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
@@ -5163,10 +5163,10 @@
         <v>0</v>
       </c>
       <c r="I118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J118" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -5203,10 +5203,10 @@
         <v>6</v>
       </c>
       <c r="I119" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J119" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
@@ -5243,10 +5243,10 @@
         <v>2</v>
       </c>
       <c r="I120" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J120" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121">
@@ -5363,10 +5363,10 @@
         <v>6</v>
       </c>
       <c r="I123" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J123" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124">
@@ -5403,10 +5403,10 @@
         <v>1</v>
       </c>
       <c r="I124" t="n">
+        <v>1</v>
+      </c>
+      <c r="J124" t="n">
         <v>3</v>
-      </c>
-      <c r="J124" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -5443,10 +5443,10 @@
         <v>13</v>
       </c>
       <c r="I125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -5483,10 +5483,10 @@
         <v>2</v>
       </c>
       <c r="I126" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J126" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127">
@@ -5523,10 +5523,10 @@
         <v>0</v>
       </c>
       <c r="I127" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J127" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -5563,10 +5563,10 @@
         <v>10</v>
       </c>
       <c r="I128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -5683,10 +5683,10 @@
         <v>3</v>
       </c>
       <c r="I131" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J131" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -5763,10 +5763,10 @@
         <v>4</v>
       </c>
       <c r="I133" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J133" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134">
@@ -5803,10 +5803,10 @@
         <v>4</v>
       </c>
       <c r="I134" t="n">
+        <v>2</v>
+      </c>
+      <c r="J134" t="n">
         <v>5</v>
-      </c>
-      <c r="J134" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="135">
@@ -5843,10 +5843,10 @@
         <v>7</v>
       </c>
       <c r="I135" t="n">
+        <v>1</v>
+      </c>
+      <c r="J135" t="n">
         <v>5</v>
-      </c>
-      <c r="J135" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="136">
@@ -5883,10 +5883,10 @@
         <v>5</v>
       </c>
       <c r="I136" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J136" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -5923,10 +5923,10 @@
         <v>6</v>
       </c>
       <c r="I137" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J137" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138">
@@ -6003,10 +6003,10 @@
         <v>5</v>
       </c>
       <c r="I139" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J139" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -6043,10 +6043,10 @@
         <v>8</v>
       </c>
       <c r="I140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" t="n">
         <v>3</v>
-      </c>
-      <c r="J140" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -6083,10 +6083,10 @@
         <v>10</v>
       </c>
       <c r="I141" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J141" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142">
@@ -6123,10 +6123,10 @@
         <v>1</v>
       </c>
       <c r="I142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -6163,10 +6163,10 @@
         <v>10</v>
       </c>
       <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" t="n">
         <v>3</v>
-      </c>
-      <c r="J143" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -6203,10 +6203,10 @@
         <v>10</v>
       </c>
       <c r="I144" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J144" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -6243,10 +6243,10 @@
         <v>16</v>
       </c>
       <c r="I145" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J145" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -6323,10 +6323,10 @@
         <v>5</v>
       </c>
       <c r="I147" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J147" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -6363,10 +6363,10 @@
         <v>4</v>
       </c>
       <c r="I148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -6443,10 +6443,10 @@
         <v>14</v>
       </c>
       <c r="I150" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
@@ -6483,10 +6483,10 @@
         <v>14</v>
       </c>
       <c r="I151" t="n">
+        <v>2</v>
+      </c>
+      <c r="J151" t="n">
         <v>5</v>
-      </c>
-      <c r="J151" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -6523,10 +6523,10 @@
         <v>3</v>
       </c>
       <c r="I152" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J152" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153">
@@ -6563,10 +6563,10 @@
         <v>8</v>
       </c>
       <c r="I153" t="n">
+        <v>6</v>
+      </c>
+      <c r="J153" t="n">
         <v>3</v>
-      </c>
-      <c r="J153" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="154">
@@ -6603,10 +6603,10 @@
         <v>1</v>
       </c>
       <c r="I154" t="n">
+        <v>5</v>
+      </c>
+      <c r="J154" t="n">
         <v>3</v>
-      </c>
-      <c r="J154" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="155">
@@ -6643,10 +6643,10 @@
         <v>0</v>
       </c>
       <c r="I155" t="n">
+        <v>0</v>
+      </c>
+      <c r="J155" t="n">
         <v>5</v>
-      </c>
-      <c r="J155" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -6683,10 +6683,10 @@
         <v>10</v>
       </c>
       <c r="I156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -6723,10 +6723,10 @@
         <v>4</v>
       </c>
       <c r="I157" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J157" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -6763,10 +6763,10 @@
         <v>14</v>
       </c>
       <c r="I158" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J158" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -6803,10 +6803,10 @@
         <v>2</v>
       </c>
       <c r="I159" t="n">
+        <v>0</v>
+      </c>
+      <c r="J159" t="n">
         <v>3</v>
-      </c>
-      <c r="J159" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -6843,10 +6843,10 @@
         <v>4</v>
       </c>
       <c r="I160" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J160" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -7003,10 +7003,10 @@
         <v>1</v>
       </c>
       <c r="I164" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J164" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165">
@@ -7043,10 +7043,10 @@
         <v>4</v>
       </c>
       <c r="I165" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J165" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166">
@@ -7083,10 +7083,10 @@
         <v>7</v>
       </c>
       <c r="I166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J166" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -7123,10 +7123,10 @@
         <v>4</v>
       </c>
       <c r="I167" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J167" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -7163,10 +7163,10 @@
         <v>12</v>
       </c>
       <c r="I168" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J168" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169">
@@ -7203,10 +7203,10 @@
         <v>2</v>
       </c>
       <c r="I169" t="n">
+        <v>0</v>
+      </c>
+      <c r="J169" t="n">
         <v>5</v>
-      </c>
-      <c r="J169" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -7323,10 +7323,10 @@
         <v>4</v>
       </c>
       <c r="I172" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
@@ -7363,10 +7363,10 @@
         <v>4</v>
       </c>
       <c r="I173" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J173" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174">
@@ -7403,10 +7403,10 @@
         <v>8</v>
       </c>
       <c r="I174" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J174" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175">
@@ -7523,10 +7523,10 @@
         <v>6</v>
       </c>
       <c r="I177" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J177" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -7563,10 +7563,10 @@
         <v>6</v>
       </c>
       <c r="I178" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J178" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179">
@@ -7643,10 +7643,10 @@
         <v>5</v>
       </c>
       <c r="I180" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J180" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
@@ -7683,10 +7683,10 @@
         <v>3</v>
       </c>
       <c r="I181" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J181" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -7723,10 +7723,10 @@
         <v>11</v>
       </c>
       <c r="I182" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J182" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183">
@@ -7763,10 +7763,10 @@
         <v>8</v>
       </c>
       <c r="I183" t="n">
+        <v>1</v>
+      </c>
+      <c r="J183" t="n">
         <v>5</v>
-      </c>
-      <c r="J183" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="184">
@@ -7803,10 +7803,10 @@
         <v>14</v>
       </c>
       <c r="I184" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J184" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -7843,10 +7843,10 @@
         <v>2</v>
       </c>
       <c r="I185" t="n">
+        <v>2</v>
+      </c>
+      <c r="J185" t="n">
         <v>3</v>
-      </c>
-      <c r="J185" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="186">
@@ -7883,10 +7883,10 @@
         <v>6</v>
       </c>
       <c r="I186" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J186" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -7923,10 +7923,10 @@
         <v>9</v>
       </c>
       <c r="I187" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J187" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="188">
@@ -7963,10 +7963,10 @@
         <v>7</v>
       </c>
       <c r="I188" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J188" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189">
@@ -8003,10 +8003,10 @@
         <v>5</v>
       </c>
       <c r="I189" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J189" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190">
@@ -8043,10 +8043,10 @@
         <v>5</v>
       </c>
       <c r="I190" t="n">
+        <v>1</v>
+      </c>
+      <c r="J190" t="n">
         <v>5</v>
-      </c>
-      <c r="J190" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -8083,10 +8083,10 @@
         <v>6</v>
       </c>
       <c r="I191" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J191" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -8123,10 +8123,10 @@
         <v>11</v>
       </c>
       <c r="I192" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J192" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193">
@@ -8203,10 +8203,10 @@
         <v>2</v>
       </c>
       <c r="I194" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J194" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
@@ -8243,10 +8243,10 @@
         <v>13</v>
       </c>
       <c r="I195" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J195" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -8283,10 +8283,10 @@
         <v>0</v>
       </c>
       <c r="I196" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J196" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -8403,10 +8403,10 @@
         <v>3</v>
       </c>
       <c r="I199" t="n">
+        <v>1</v>
+      </c>
+      <c r="J199" t="n">
         <v>3</v>
-      </c>
-      <c r="J199" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -8443,10 +8443,10 @@
         <v>3</v>
       </c>
       <c r="I200" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J200" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="201">
@@ -8483,10 +8483,10 @@
         <v>0</v>
       </c>
       <c r="I201" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J201" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">
@@ -8563,10 +8563,10 @@
         <v>3</v>
       </c>
       <c r="I203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">
@@ -8603,10 +8603,10 @@
         <v>12</v>
       </c>
       <c r="I204" t="n">
+        <v>0</v>
+      </c>
+      <c r="J204" t="n">
         <v>3</v>
-      </c>
-      <c r="J204" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="205">
@@ -8643,10 +8643,10 @@
         <v>6</v>
       </c>
       <c r="I205" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J205" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="206">
@@ -8683,10 +8683,10 @@
         <v>4</v>
       </c>
       <c r="I206" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J206" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="207">
@@ -8723,10 +8723,10 @@
         <v>6</v>
       </c>
       <c r="I207" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J207" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208">
@@ -8763,10 +8763,10 @@
         <v>1</v>
       </c>
       <c r="I208" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J208" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="209">
@@ -8843,10 +8843,10 @@
         <v>13</v>
       </c>
       <c r="I210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -8883,10 +8883,10 @@
         <v>5</v>
       </c>
       <c r="I211" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J211" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -8963,10 +8963,10 @@
         <v>6</v>
       </c>
       <c r="I213" t="n">
+        <v>1</v>
+      </c>
+      <c r="J213" t="n">
         <v>5</v>
-      </c>
-      <c r="J213" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="214">
@@ -9003,10 +9003,10 @@
         <v>1</v>
       </c>
       <c r="I214" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J214" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
@@ -9043,10 +9043,10 @@
         <v>16</v>
       </c>
       <c r="I215" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J215" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216">
@@ -9083,10 +9083,10 @@
         <v>2</v>
       </c>
       <c r="I216" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J216" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="217">
@@ -9123,10 +9123,10 @@
         <v>1</v>
       </c>
       <c r="I217" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J217" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="218">
@@ -9283,10 +9283,10 @@
         <v>4</v>
       </c>
       <c r="I221" t="n">
+        <v>3</v>
+      </c>
+      <c r="J221" t="n">
         <v>6</v>
-      </c>
-      <c r="J221" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="222">
@@ -9323,10 +9323,10 @@
         <v>3</v>
       </c>
       <c r="I222" t="n">
+        <v>2</v>
+      </c>
+      <c r="J222" t="n">
         <v>3</v>
-      </c>
-      <c r="J222" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="223">
@@ -9363,10 +9363,10 @@
         <v>9</v>
       </c>
       <c r="I223" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J223" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224">
@@ -9403,10 +9403,10 @@
         <v>1</v>
       </c>
       <c r="I224" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J224" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225">
@@ -9443,10 +9443,10 @@
         <v>7</v>
       </c>
       <c r="I225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -9483,10 +9483,10 @@
         <v>2</v>
       </c>
       <c r="I226" t="n">
+        <v>1</v>
+      </c>
+      <c r="J226" t="n">
         <v>9</v>
-      </c>
-      <c r="J226" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="227">
@@ -9523,10 +9523,10 @@
         <v>5</v>
       </c>
       <c r="I227" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J227" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228">
@@ -9563,10 +9563,10 @@
         <v>1</v>
       </c>
       <c r="I228" t="n">
+        <v>1</v>
+      </c>
+      <c r="J228" t="n">
         <v>3</v>
-      </c>
-      <c r="J228" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -9603,10 +9603,10 @@
         <v>0</v>
       </c>
       <c r="I229" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J229" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="230">
@@ -9643,10 +9643,10 @@
         <v>9</v>
       </c>
       <c r="I230" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J230" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete stat order overhaul: PTS/REB/AST/STL/BLK throughout entire system
- Regenerated master database with new bucket structure (points, rebounds, assists, steals, blocks)
- Updated all Python backend files to generate stats in new order
- Fixed fast_daily_pipeline.py to parse stats correctly
- Updated all frontend components to display stats in correct order
- Fixed bucket search API to construct bucket_key in new order
- Reordered sliders in bucket search page
- Updated GameCard, RecentGameCard, and UltimateChartCard components
- All stat displays now consistent: PTS/REB/AST/STL/BLK
</commit_message>
<xml_diff>
--- a/CurrentSeason_UniqornGames_Master.xlsx
+++ b/CurrentSeason_UniqornGames_Master.xlsx
@@ -517,16 +517,16 @@
         <v>25</v>
       </c>
       <c r="G2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="n">
         <v>14</v>
       </c>
-      <c r="H2" t="n">
-        <v>6</v>
-      </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -557,16 +557,16 @@
         <v>41</v>
       </c>
       <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
         <v>8</v>
       </c>
-      <c r="H3" t="n">
-        <v>2</v>
-      </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -597,16 +597,16 @@
         <v>22</v>
       </c>
       <c r="G4" t="n">
+        <v>17</v>
+      </c>
+      <c r="H4" t="n">
         <v>14</v>
       </c>
-      <c r="H4" t="n">
-        <v>17</v>
-      </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -637,16 +637,16 @@
         <v>12</v>
       </c>
       <c r="G5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H5" t="n">
         <v>7</v>
       </c>
-      <c r="H5" t="n">
-        <v>6</v>
-      </c>
       <c r="I5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -677,10 +677,10 @@
         <v>17</v>
       </c>
       <c r="G6" t="n">
+        <v>11</v>
+      </c>
+      <c r="H6" t="n">
         <v>12</v>
-      </c>
-      <c r="H6" t="n">
-        <v>11</v>
       </c>
       <c r="I6" t="n">
         <v>3</v>
@@ -717,10 +717,10 @@
         <v>3</v>
       </c>
       <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" t="n">
         <v>14</v>
-      </c>
-      <c r="H7" t="n">
-        <v>6</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -763,10 +763,10 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
         <v>6</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -797,16 +797,16 @@
         <v>21</v>
       </c>
       <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
         <v>3</v>
       </c>
-      <c r="H9" t="n">
-        <v>5</v>
-      </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -837,16 +837,16 @@
         <v>26</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -877,16 +877,16 @@
         <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -917,16 +917,16 @@
         <v>31</v>
       </c>
       <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
         <v>3</v>
       </c>
-      <c r="H12" t="n">
-        <v>1</v>
-      </c>
       <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
         <v>5</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -963,10 +963,10 @@
         <v>11</v>
       </c>
       <c r="I13" t="n">
+        <v>4</v>
+      </c>
+      <c r="J13" t="n">
         <v>3</v>
-      </c>
-      <c r="J13" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -997,16 +997,16 @@
         <v>22</v>
       </c>
       <c r="G14" t="n">
+        <v>15</v>
+      </c>
+      <c r="H14" t="n">
         <v>16</v>
       </c>
-      <c r="H14" t="n">
-        <v>15</v>
-      </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1037,16 +1037,16 @@
         <v>29</v>
       </c>
       <c r="G15" t="n">
+        <v>9</v>
+      </c>
+      <c r="H15" t="n">
         <v>5</v>
       </c>
-      <c r="H15" t="n">
-        <v>9</v>
-      </c>
       <c r="I15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -1077,16 +1077,16 @@
         <v>42</v>
       </c>
       <c r="G16" t="n">
+        <v>9</v>
+      </c>
+      <c r="H16" t="n">
         <v>8</v>
       </c>
-      <c r="H16" t="n">
-        <v>9</v>
-      </c>
       <c r="I16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1117,16 +1117,16 @@
         <v>10</v>
       </c>
       <c r="G17" t="n">
+        <v>2</v>
+      </c>
+      <c r="H17" t="n">
         <v>19</v>
       </c>
-      <c r="H17" t="n">
-        <v>2</v>
-      </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J17" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1157,16 +1157,16 @@
         <v>18</v>
       </c>
       <c r="G18" t="n">
+        <v>9</v>
+      </c>
+      <c r="H18" t="n">
         <v>6</v>
       </c>
-      <c r="H18" t="n">
-        <v>9</v>
-      </c>
       <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
         <v>5</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1197,16 +1197,16 @@
         <v>16</v>
       </c>
       <c r="G19" t="n">
+        <v>5</v>
+      </c>
+      <c r="H19" t="n">
         <v>16</v>
       </c>
-      <c r="H19" t="n">
-        <v>5</v>
-      </c>
       <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
         <v>3</v>
-      </c>
-      <c r="J19" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1237,16 +1237,16 @@
         <v>22</v>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J20" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1277,16 +1277,16 @@
         <v>17</v>
       </c>
       <c r="G21" t="n">
+        <v>22</v>
+      </c>
+      <c r="H21" t="n">
         <v>5</v>
       </c>
-      <c r="H21" t="n">
-        <v>22</v>
-      </c>
       <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
         <v>3</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1317,16 +1317,16 @@
         <v>32</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H22" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1357,16 +1357,16 @@
         <v>26</v>
       </c>
       <c r="G23" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" t="n">
         <v>16</v>
       </c>
-      <c r="H23" t="n">
-        <v>2</v>
-      </c>
       <c r="I23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -1397,16 +1397,16 @@
         <v>18</v>
       </c>
       <c r="G24" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H24" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -1437,16 +1437,16 @@
         <v>8</v>
       </c>
       <c r="G25" t="n">
+        <v>5</v>
+      </c>
+      <c r="H25" t="n">
         <v>12</v>
       </c>
-      <c r="H25" t="n">
-        <v>5</v>
-      </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1477,16 +1477,16 @@
         <v>3</v>
       </c>
       <c r="G26" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H26" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I26" t="n">
+        <v>2</v>
+      </c>
+      <c r="J26" t="n">
         <v>5</v>
-      </c>
-      <c r="J26" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -1517,16 +1517,16 @@
         <v>40</v>
       </c>
       <c r="G27" t="n">
+        <v>5</v>
+      </c>
+      <c r="H27" t="n">
         <v>17</v>
       </c>
-      <c r="H27" t="n">
-        <v>5</v>
-      </c>
       <c r="I27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J27" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1557,16 +1557,16 @@
         <v>34</v>
       </c>
       <c r="G28" t="n">
+        <v>13</v>
+      </c>
+      <c r="H28" t="n">
         <v>5</v>
       </c>
-      <c r="H28" t="n">
-        <v>13</v>
-      </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1597,16 +1597,16 @@
         <v>7</v>
       </c>
       <c r="G29" t="n">
+        <v>3</v>
+      </c>
+      <c r="H29" t="n">
         <v>8</v>
       </c>
-      <c r="H29" t="n">
-        <v>3</v>
-      </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J29" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1637,10 +1637,10 @@
         <v>9</v>
       </c>
       <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
         <v>16</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0</v>
       </c>
       <c r="I30" t="n">
         <v>2</v>
@@ -1677,16 +1677,16 @@
         <v>7</v>
       </c>
       <c r="G31" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H31" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1717,16 +1717,16 @@
         <v>16</v>
       </c>
       <c r="G32" t="n">
+        <v>2</v>
+      </c>
+      <c r="H32" t="n">
         <v>9</v>
       </c>
-      <c r="H32" t="n">
-        <v>2</v>
-      </c>
       <c r="I32" t="n">
+        <v>2</v>
+      </c>
+      <c r="J32" t="n">
         <v>6</v>
-      </c>
-      <c r="J32" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -1757,16 +1757,16 @@
         <v>7</v>
       </c>
       <c r="G33" t="n">
+        <v>2</v>
+      </c>
+      <c r="H33" t="n">
         <v>8</v>
       </c>
-      <c r="H33" t="n">
-        <v>2</v>
-      </c>
       <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
         <v>6</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1797,16 +1797,16 @@
         <v>21</v>
       </c>
       <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="n">
         <v>14</v>
       </c>
-      <c r="H34" t="n">
-        <v>1</v>
-      </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J34" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1837,16 +1837,16 @@
         <v>15</v>
       </c>
       <c r="G35" t="n">
+        <v>9</v>
+      </c>
+      <c r="H35" t="n">
         <v>6</v>
       </c>
-      <c r="H35" t="n">
-        <v>9</v>
-      </c>
       <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
         <v>5</v>
-      </c>
-      <c r="J35" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1877,16 +1877,16 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H36" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1917,16 +1917,16 @@
         <v>4</v>
       </c>
       <c r="G37" t="n">
+        <v>4</v>
+      </c>
+      <c r="H37" t="n">
         <v>5</v>
       </c>
-      <c r="H37" t="n">
-        <v>4</v>
-      </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J37" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1957,16 +1957,16 @@
         <v>26</v>
       </c>
       <c r="G38" t="n">
+        <v>5</v>
+      </c>
+      <c r="H38" t="n">
         <v>7</v>
       </c>
-      <c r="H38" t="n">
-        <v>5</v>
-      </c>
       <c r="I38" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -1997,16 +1997,16 @@
         <v>28</v>
       </c>
       <c r="G39" t="n">
+        <v>3</v>
+      </c>
+      <c r="H39" t="n">
         <v>16</v>
       </c>
-      <c r="H39" t="n">
-        <v>3</v>
-      </c>
       <c r="I39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J39" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -2037,16 +2037,16 @@
         <v>26</v>
       </c>
       <c r="G40" t="n">
+        <v>5</v>
+      </c>
+      <c r="H40" t="n">
         <v>3</v>
       </c>
-      <c r="H40" t="n">
-        <v>5</v>
-      </c>
       <c r="I40" t="n">
+        <v>2</v>
+      </c>
+      <c r="J40" t="n">
         <v>6</v>
-      </c>
-      <c r="J40" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -2077,16 +2077,16 @@
         <v>8</v>
       </c>
       <c r="G41" t="n">
+        <v>2</v>
+      </c>
+      <c r="H41" t="n">
         <v>22</v>
       </c>
-      <c r="H41" t="n">
-        <v>2</v>
-      </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2117,16 +2117,16 @@
         <v>16</v>
       </c>
       <c r="G42" t="n">
+        <v>10</v>
+      </c>
+      <c r="H42" t="n">
         <v>3</v>
       </c>
-      <c r="H42" t="n">
-        <v>10</v>
-      </c>
       <c r="I42" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
@@ -2157,16 +2157,16 @@
         <v>29</v>
       </c>
       <c r="G43" t="n">
+        <v>3</v>
+      </c>
+      <c r="H43" t="n">
         <v>12</v>
       </c>
-      <c r="H43" t="n">
-        <v>3</v>
-      </c>
       <c r="I43" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J43" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -2197,16 +2197,16 @@
         <v>20</v>
       </c>
       <c r="G44" t="n">
+        <v>3</v>
+      </c>
+      <c r="H44" t="n">
         <v>14</v>
       </c>
-      <c r="H44" t="n">
-        <v>3</v>
-      </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J44" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -2237,10 +2237,10 @@
         <v>5</v>
       </c>
       <c r="G45" t="n">
+        <v>13</v>
+      </c>
+      <c r="H45" t="n">
         <v>5</v>
-      </c>
-      <c r="H45" t="n">
-        <v>13</v>
       </c>
       <c r="I45" t="n">
         <v>1</v>
@@ -2277,16 +2277,16 @@
         <v>4</v>
       </c>
       <c r="G46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
         <v>6</v>
-      </c>
-      <c r="J46" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2317,16 +2317,16 @@
         <v>16</v>
       </c>
       <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
         <v>16</v>
       </c>
-      <c r="H47" t="n">
-        <v>0</v>
-      </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J47" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2357,16 +2357,16 @@
         <v>10</v>
       </c>
       <c r="G48" t="n">
+        <v>8</v>
+      </c>
+      <c r="H48" t="n">
         <v>11</v>
       </c>
-      <c r="H48" t="n">
-        <v>8</v>
-      </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J48" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2397,16 +2397,16 @@
         <v>29</v>
       </c>
       <c r="G49" t="n">
+        <v>7</v>
+      </c>
+      <c r="H49" t="n">
         <v>13</v>
       </c>
-      <c r="H49" t="n">
-        <v>7</v>
-      </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J49" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2437,16 +2437,16 @@
         <v>15</v>
       </c>
       <c r="G50" t="n">
+        <v>4</v>
+      </c>
+      <c r="H50" t="n">
         <v>9</v>
       </c>
-      <c r="H50" t="n">
-        <v>4</v>
-      </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J50" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2477,16 +2477,16 @@
         <v>13</v>
       </c>
       <c r="G51" t="n">
+        <v>2</v>
+      </c>
+      <c r="H51" t="n">
         <v>16</v>
       </c>
-      <c r="H51" t="n">
-        <v>2</v>
-      </c>
       <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
         <v>3</v>
-      </c>
-      <c r="J51" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2517,16 +2517,16 @@
         <v>35</v>
       </c>
       <c r="G52" t="n">
+        <v>3</v>
+      </c>
+      <c r="H52" t="n">
         <v>8</v>
       </c>
-      <c r="H52" t="n">
-        <v>3</v>
-      </c>
       <c r="I52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J52" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -2557,16 +2557,16 @@
         <v>7</v>
       </c>
       <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="n">
         <v>5</v>
       </c>
-      <c r="H53" t="n">
-        <v>1</v>
-      </c>
       <c r="I53" t="n">
+        <v>4</v>
+      </c>
+      <c r="J53" t="n">
         <v>3</v>
-      </c>
-      <c r="J53" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="54">
@@ -2597,16 +2597,16 @@
         <v>2</v>
       </c>
       <c r="G54" t="n">
+        <v>3</v>
+      </c>
+      <c r="H54" t="n">
         <v>13</v>
       </c>
-      <c r="H54" t="n">
-        <v>3</v>
-      </c>
       <c r="I54" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J54" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -2637,16 +2637,16 @@
         <v>23</v>
       </c>
       <c r="G55" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H55" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2677,16 +2677,16 @@
         <v>20</v>
       </c>
       <c r="G56" t="n">
+        <v>9</v>
+      </c>
+      <c r="H56" t="n">
         <v>13</v>
       </c>
-      <c r="H56" t="n">
-        <v>9</v>
-      </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2717,16 +2717,16 @@
         <v>29</v>
       </c>
       <c r="G57" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H57" t="n">
+        <v>4</v>
+      </c>
+      <c r="I57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" t="n">
         <v>8</v>
-      </c>
-      <c r="I57" t="n">
-        <v>8</v>
-      </c>
-      <c r="J57" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -2757,16 +2757,16 @@
         <v>16</v>
       </c>
       <c r="G58" t="n">
+        <v>14</v>
+      </c>
+      <c r="H58" t="n">
         <v>3</v>
       </c>
-      <c r="H58" t="n">
-        <v>14</v>
-      </c>
       <c r="I58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2797,16 +2797,16 @@
         <v>28</v>
       </c>
       <c r="G59" t="n">
+        <v>6</v>
+      </c>
+      <c r="H59" t="n">
         <v>16</v>
       </c>
-      <c r="H59" t="n">
-        <v>6</v>
-      </c>
       <c r="I59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2837,10 +2837,10 @@
         <v>42</v>
       </c>
       <c r="G60" t="n">
+        <v>6</v>
+      </c>
+      <c r="H60" t="n">
         <v>3</v>
-      </c>
-      <c r="H60" t="n">
-        <v>6</v>
       </c>
       <c r="I60" t="n">
         <v>2</v>
@@ -2877,10 +2877,10 @@
         <v>55</v>
       </c>
       <c r="G61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H61" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
@@ -2917,16 +2917,16 @@
         <v>22</v>
       </c>
       <c r="G62" t="n">
+        <v>9</v>
+      </c>
+      <c r="H62" t="n">
         <v>5</v>
       </c>
-      <c r="H62" t="n">
-        <v>9</v>
-      </c>
       <c r="I62" t="n">
+        <v>2</v>
+      </c>
+      <c r="J62" t="n">
         <v>5</v>
-      </c>
-      <c r="J62" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -2957,16 +2957,16 @@
         <v>19</v>
       </c>
       <c r="G63" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H63" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I63" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64">
@@ -2997,10 +2997,10 @@
         <v>30</v>
       </c>
       <c r="G64" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" t="n">
         <v>3</v>
-      </c>
-      <c r="H64" t="n">
-        <v>1</v>
       </c>
       <c r="I64" t="n">
         <v>2</v>
@@ -3037,16 +3037,16 @@
         <v>26</v>
       </c>
       <c r="G65" t="n">
+        <v>4</v>
+      </c>
+      <c r="H65" t="n">
         <v>13</v>
       </c>
-      <c r="H65" t="n">
-        <v>4</v>
-      </c>
       <c r="I65" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J65" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -3077,16 +3077,16 @@
         <v>10</v>
       </c>
       <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
         <v>3</v>
       </c>
-      <c r="H66" t="n">
-        <v>0</v>
-      </c>
       <c r="I66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" t="n">
         <v>6</v>
-      </c>
-      <c r="J66" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -3117,16 +3117,16 @@
         <v>26</v>
       </c>
       <c r="G67" t="n">
+        <v>13</v>
+      </c>
+      <c r="H67" t="n">
         <v>7</v>
       </c>
-      <c r="H67" t="n">
-        <v>13</v>
-      </c>
       <c r="I67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -3163,10 +3163,10 @@
         <v>5</v>
       </c>
       <c r="I68" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J68" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -3197,16 +3197,16 @@
         <v>6</v>
       </c>
       <c r="G69" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H69" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I69" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -3237,16 +3237,16 @@
         <v>5</v>
       </c>
       <c r="G70" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H70" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
         <v>5</v>
-      </c>
-      <c r="J70" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -3277,16 +3277,16 @@
         <v>14</v>
       </c>
       <c r="G71" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" t="n">
         <v>13</v>
       </c>
-      <c r="H71" t="n">
-        <v>1</v>
-      </c>
       <c r="I71" t="n">
+        <v>2</v>
+      </c>
+      <c r="J71" t="n">
         <v>3</v>
-      </c>
-      <c r="J71" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -3317,10 +3317,10 @@
         <v>17</v>
       </c>
       <c r="G72" t="n">
+        <v>3</v>
+      </c>
+      <c r="H72" t="n">
         <v>15</v>
-      </c>
-      <c r="H72" t="n">
-        <v>3</v>
       </c>
       <c r="I72" t="n">
         <v>3</v>
@@ -3357,16 +3357,16 @@
         <v>2</v>
       </c>
       <c r="G73" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H73" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I73" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74">
@@ -3397,16 +3397,16 @@
         <v>26</v>
       </c>
       <c r="G74" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" t="n">
         <v>8</v>
       </c>
-      <c r="H74" t="n">
-        <v>1</v>
-      </c>
       <c r="I74" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75">
@@ -3437,16 +3437,16 @@
         <v>27</v>
       </c>
       <c r="G75" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H75" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -3477,16 +3477,16 @@
         <v>14</v>
       </c>
       <c r="G76" t="n">
+        <v>12</v>
+      </c>
+      <c r="H76" t="n">
         <v>16</v>
       </c>
-      <c r="H76" t="n">
-        <v>12</v>
-      </c>
       <c r="I76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -3517,16 +3517,16 @@
         <v>17</v>
       </c>
       <c r="G77" t="n">
+        <v>10</v>
+      </c>
+      <c r="H77" t="n">
         <v>11</v>
       </c>
-      <c r="H77" t="n">
-        <v>10</v>
-      </c>
       <c r="I77" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J77" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -3557,16 +3557,16 @@
         <v>2</v>
       </c>
       <c r="G78" t="n">
+        <v>15</v>
+      </c>
+      <c r="H78" t="n">
         <v>6</v>
       </c>
-      <c r="H78" t="n">
-        <v>15</v>
-      </c>
       <c r="I78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -3597,16 +3597,16 @@
         <v>10</v>
       </c>
       <c r="G79" t="n">
+        <v>6</v>
+      </c>
+      <c r="H79" t="n">
         <v>11</v>
       </c>
-      <c r="H79" t="n">
-        <v>6</v>
-      </c>
       <c r="I79" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80">
@@ -3637,16 +3637,16 @@
         <v>16</v>
       </c>
       <c r="G80" t="n">
+        <v>2</v>
+      </c>
+      <c r="H80" t="n">
         <v>14</v>
       </c>
-      <c r="H80" t="n">
-        <v>2</v>
-      </c>
       <c r="I80" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J80" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
@@ -3677,10 +3677,10 @@
         <v>7</v>
       </c>
       <c r="G81" t="n">
+        <v>4</v>
+      </c>
+      <c r="H81" t="n">
         <v>11</v>
-      </c>
-      <c r="H81" t="n">
-        <v>4</v>
       </c>
       <c r="I81" t="n">
         <v>2</v>
@@ -3723,10 +3723,10 @@
         <v>9</v>
       </c>
       <c r="I82" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -3757,16 +3757,16 @@
         <v>29</v>
       </c>
       <c r="G83" t="n">
+        <v>13</v>
+      </c>
+      <c r="H83" t="n">
         <v>3</v>
       </c>
-      <c r="H83" t="n">
-        <v>13</v>
-      </c>
       <c r="I83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -3803,10 +3803,10 @@
         <v>6</v>
       </c>
       <c r="I84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J84" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85">
@@ -3837,16 +3837,16 @@
         <v>27</v>
       </c>
       <c r="G85" t="n">
+        <v>10</v>
+      </c>
+      <c r="H85" t="n">
         <v>3</v>
       </c>
-      <c r="H85" t="n">
-        <v>10</v>
-      </c>
       <c r="I85" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J85" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -3877,16 +3877,16 @@
         <v>21</v>
       </c>
       <c r="G86" t="n">
+        <v>3</v>
+      </c>
+      <c r="H86" t="n">
         <v>6</v>
       </c>
-      <c r="H86" t="n">
+      <c r="I86" t="n">
         <v>3</v>
       </c>
-      <c r="I86" t="n">
-        <v>4</v>
-      </c>
       <c r="J86" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -3917,10 +3917,10 @@
         <v>20</v>
       </c>
       <c r="G87" t="n">
+        <v>12</v>
+      </c>
+      <c r="H87" t="n">
         <v>5</v>
-      </c>
-      <c r="H87" t="n">
-        <v>12</v>
       </c>
       <c r="I87" t="n">
         <v>2</v>
@@ -3957,16 +3957,16 @@
         <v>13</v>
       </c>
       <c r="G88" t="n">
+        <v>8</v>
+      </c>
+      <c r="H88" t="n">
         <v>12</v>
       </c>
-      <c r="H88" t="n">
-        <v>8</v>
-      </c>
       <c r="I88" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J88" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3997,10 +3997,10 @@
         <v>26</v>
       </c>
       <c r="G89" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H89" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I89" t="n">
         <v>2</v>
@@ -4037,16 +4037,16 @@
         <v>23</v>
       </c>
       <c r="G90" t="n">
+        <v>3</v>
+      </c>
+      <c r="H90" t="n">
         <v>8</v>
       </c>
-      <c r="H90" t="n">
-        <v>3</v>
-      </c>
       <c r="I90" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J90" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -4077,16 +4077,16 @@
         <v>8</v>
       </c>
       <c r="G91" t="n">
+        <v>4</v>
+      </c>
+      <c r="H91" t="n">
         <v>16</v>
       </c>
-      <c r="H91" t="n">
-        <v>4</v>
-      </c>
       <c r="I91" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J91" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -4117,10 +4117,10 @@
         <v>45</v>
       </c>
       <c r="G92" t="n">
+        <v>3</v>
+      </c>
+      <c r="H92" t="n">
         <v>7</v>
-      </c>
-      <c r="H92" t="n">
-        <v>3</v>
       </c>
       <c r="I92" t="n">
         <v>2</v>
@@ -4157,10 +4157,10 @@
         <v>4</v>
       </c>
       <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
         <v>13</v>
-      </c>
-      <c r="H93" t="n">
-        <v>0</v>
       </c>
       <c r="I93" t="n">
         <v>2</v>
@@ -4197,16 +4197,16 @@
         <v>12</v>
       </c>
       <c r="G94" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" t="n">
         <v>10</v>
       </c>
-      <c r="H94" t="n">
-        <v>1</v>
-      </c>
       <c r="I94" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J94" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -4237,16 +4237,16 @@
         <v>9</v>
       </c>
       <c r="G95" t="n">
+        <v>4</v>
+      </c>
+      <c r="H95" t="n">
         <v>7</v>
       </c>
-      <c r="H95" t="n">
-        <v>4</v>
-      </c>
       <c r="I95" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J95" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
@@ -4277,16 +4277,16 @@
         <v>27</v>
       </c>
       <c r="G96" t="n">
+        <v>6</v>
+      </c>
+      <c r="H96" t="n">
         <v>7</v>
       </c>
-      <c r="H96" t="n">
-        <v>6</v>
-      </c>
       <c r="I96" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J96" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -4317,10 +4317,10 @@
         <v>28</v>
       </c>
       <c r="G97" t="n">
+        <v>4</v>
+      </c>
+      <c r="H97" t="n">
         <v>16</v>
-      </c>
-      <c r="H97" t="n">
-        <v>4</v>
       </c>
       <c r="I97" t="n">
         <v>0</v>
@@ -4357,16 +4357,16 @@
         <v>23</v>
       </c>
       <c r="G98" t="n">
+        <v>10</v>
+      </c>
+      <c r="H98" t="n">
         <v>25</v>
       </c>
-      <c r="H98" t="n">
-        <v>10</v>
-      </c>
       <c r="I98" t="n">
+        <v>1</v>
+      </c>
+      <c r="J98" t="n">
         <v>3</v>
-      </c>
-      <c r="J98" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -4397,16 +4397,16 @@
         <v>55</v>
       </c>
       <c r="G99" t="n">
+        <v>2</v>
+      </c>
+      <c r="H99" t="n">
         <v>11</v>
       </c>
-      <c r="H99" t="n">
-        <v>2</v>
-      </c>
       <c r="I99" t="n">
+        <v>3</v>
+      </c>
+      <c r="J99" t="n">
         <v>5</v>
-      </c>
-      <c r="J99" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="100">
@@ -4437,16 +4437,16 @@
         <v>20</v>
       </c>
       <c r="G100" t="n">
+        <v>1</v>
+      </c>
+      <c r="H100" t="n">
         <v>9</v>
       </c>
-      <c r="H100" t="n">
-        <v>1</v>
-      </c>
       <c r="I100" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J100" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
@@ -4477,16 +4477,16 @@
         <v>28</v>
       </c>
       <c r="G101" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H101" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I101" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J101" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102">
@@ -4517,16 +4517,16 @@
         <v>29</v>
       </c>
       <c r="G102" t="n">
+        <v>1</v>
+      </c>
+      <c r="H102" t="n">
         <v>9</v>
       </c>
-      <c r="H102" t="n">
-        <v>1</v>
-      </c>
       <c r="I102" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J102" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -4557,16 +4557,16 @@
         <v>8</v>
       </c>
       <c r="G103" t="n">
+        <v>9</v>
+      </c>
+      <c r="H103" t="n">
         <v>6</v>
       </c>
-      <c r="H103" t="n">
-        <v>9</v>
-      </c>
       <c r="I103" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J103" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104">
@@ -4597,16 +4597,16 @@
         <v>4</v>
       </c>
       <c r="G104" t="n">
+        <v>1</v>
+      </c>
+      <c r="H104" t="n">
         <v>8</v>
       </c>
-      <c r="H104" t="n">
-        <v>1</v>
-      </c>
       <c r="I104" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J104" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105">
@@ -4637,16 +4637,16 @@
         <v>32</v>
       </c>
       <c r="G105" t="n">
+        <v>3</v>
+      </c>
+      <c r="H105" t="n">
         <v>7</v>
       </c>
-      <c r="H105" t="n">
-        <v>3</v>
-      </c>
       <c r="I105" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J105" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -4677,10 +4677,10 @@
         <v>29</v>
       </c>
       <c r="G106" t="n">
+        <v>17</v>
+      </c>
+      <c r="H106" t="n">
         <v>5</v>
-      </c>
-      <c r="H106" t="n">
-        <v>17</v>
       </c>
       <c r="I106" t="n">
         <v>2</v>
@@ -4717,16 +4717,16 @@
         <v>30</v>
       </c>
       <c r="G107" t="n">
+        <v>4</v>
+      </c>
+      <c r="H107" t="n">
         <v>3</v>
       </c>
-      <c r="H107" t="n">
-        <v>4</v>
-      </c>
       <c r="I107" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108">
@@ -4757,16 +4757,16 @@
         <v>9</v>
       </c>
       <c r="G108" t="n">
+        <v>0</v>
+      </c>
+      <c r="H108" t="n">
         <v>12</v>
       </c>
-      <c r="H108" t="n">
-        <v>0</v>
-      </c>
       <c r="I108" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J108" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -4797,16 +4797,16 @@
         <v>22</v>
       </c>
       <c r="G109" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H109" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="I109" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J109" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110">
@@ -4837,16 +4837,16 @@
         <v>23</v>
       </c>
       <c r="G110" t="n">
+        <v>14</v>
+      </c>
+      <c r="H110" t="n">
         <v>7</v>
       </c>
-      <c r="H110" t="n">
-        <v>14</v>
-      </c>
       <c r="I110" t="n">
+        <v>0</v>
+      </c>
+      <c r="J110" t="n">
         <v>5</v>
-      </c>
-      <c r="J110" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -4877,10 +4877,10 @@
         <v>23</v>
       </c>
       <c r="G111" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H111" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I111" t="n">
         <v>3</v>
@@ -4917,16 +4917,16 @@
         <v>4</v>
       </c>
       <c r="G112" t="n">
+        <v>10</v>
+      </c>
+      <c r="H112" t="n">
         <v>3</v>
       </c>
-      <c r="H112" t="n">
-        <v>10</v>
-      </c>
       <c r="I112" t="n">
+        <v>0</v>
+      </c>
+      <c r="J112" t="n">
         <v>5</v>
-      </c>
-      <c r="J112" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -4963,10 +4963,10 @@
         <v>2</v>
       </c>
       <c r="I113" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J113" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114">
@@ -4997,16 +4997,16 @@
         <v>19</v>
       </c>
       <c r="G114" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H114" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I114" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J114" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -5037,16 +5037,16 @@
         <v>2</v>
       </c>
       <c r="G115" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H115" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I115" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J115" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
@@ -5077,10 +5077,10 @@
         <v>35</v>
       </c>
       <c r="G116" t="n">
+        <v>2</v>
+      </c>
+      <c r="H116" t="n">
         <v>17</v>
-      </c>
-      <c r="H116" t="n">
-        <v>2</v>
       </c>
       <c r="I116" t="n">
         <v>1</v>
@@ -5117,16 +5117,16 @@
         <v>24</v>
       </c>
       <c r="G117" t="n">
+        <v>9</v>
+      </c>
+      <c r="H117" t="n">
         <v>10</v>
       </c>
-      <c r="H117" t="n">
-        <v>9</v>
-      </c>
       <c r="I117" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J117" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118">
@@ -5157,16 +5157,16 @@
         <v>28</v>
       </c>
       <c r="G118" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" t="n">
         <v>19</v>
       </c>
-      <c r="H118" t="n">
-        <v>0</v>
-      </c>
       <c r="I118" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -5197,16 +5197,16 @@
         <v>28</v>
       </c>
       <c r="G119" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H119" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I119" t="n">
+        <v>2</v>
+      </c>
+      <c r="J119" t="n">
         <v>3</v>
-      </c>
-      <c r="J119" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="120">
@@ -5237,16 +5237,16 @@
         <v>14</v>
       </c>
       <c r="G120" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H120" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I120" t="n">
+        <v>4</v>
+      </c>
+      <c r="J120" t="n">
         <v>3</v>
-      </c>
-      <c r="J120" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="121">
@@ -5277,10 +5277,10 @@
         <v>8</v>
       </c>
       <c r="G121" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H121" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I121" t="n">
         <v>2</v>
@@ -5317,10 +5317,10 @@
         <v>35</v>
       </c>
       <c r="G122" t="n">
+        <v>7</v>
+      </c>
+      <c r="H122" t="n">
         <v>5</v>
-      </c>
-      <c r="H122" t="n">
-        <v>7</v>
       </c>
       <c r="I122" t="n">
         <v>2</v>
@@ -5357,16 +5357,16 @@
         <v>33</v>
       </c>
       <c r="G123" t="n">
+        <v>6</v>
+      </c>
+      <c r="H123" t="n">
         <v>5</v>
       </c>
-      <c r="H123" t="n">
-        <v>6</v>
-      </c>
       <c r="I123" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J123" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -5397,16 +5397,16 @@
         <v>8</v>
       </c>
       <c r="G124" t="n">
+        <v>1</v>
+      </c>
+      <c r="H124" t="n">
         <v>17</v>
       </c>
-      <c r="H124" t="n">
-        <v>1</v>
-      </c>
       <c r="I124" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J124" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -5437,16 +5437,16 @@
         <v>28</v>
       </c>
       <c r="G125" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H125" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="I125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
@@ -5477,16 +5477,16 @@
         <v>17</v>
       </c>
       <c r="G126" t="n">
+        <v>2</v>
+      </c>
+      <c r="H126" t="n">
         <v>3</v>
       </c>
-      <c r="H126" t="n">
-        <v>2</v>
-      </c>
       <c r="I126" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J126" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127">
@@ -5517,16 +5517,16 @@
         <v>2</v>
       </c>
       <c r="G127" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" t="n">
         <v>13</v>
       </c>
-      <c r="H127" t="n">
-        <v>0</v>
-      </c>
       <c r="I127" t="n">
+        <v>1</v>
+      </c>
+      <c r="J127" t="n">
         <v>5</v>
-      </c>
-      <c r="J127" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -5557,16 +5557,16 @@
         <v>26</v>
       </c>
       <c r="G128" t="n">
+        <v>10</v>
+      </c>
+      <c r="H128" t="n">
         <v>16</v>
       </c>
-      <c r="H128" t="n">
-        <v>10</v>
-      </c>
       <c r="I128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -5597,10 +5597,10 @@
         <v>32</v>
       </c>
       <c r="G129" t="n">
+        <v>6</v>
+      </c>
+      <c r="H129" t="n">
         <v>7</v>
-      </c>
-      <c r="H129" t="n">
-        <v>6</v>
       </c>
       <c r="I129" t="n">
         <v>2</v>
@@ -5637,10 +5637,10 @@
         <v>24</v>
       </c>
       <c r="G130" t="n">
+        <v>2</v>
+      </c>
+      <c r="H130" t="n">
         <v>11</v>
-      </c>
-      <c r="H130" t="n">
-        <v>2</v>
       </c>
       <c r="I130" t="n">
         <v>2</v>
@@ -5683,10 +5683,10 @@
         <v>3</v>
       </c>
       <c r="I131" t="n">
+        <v>1</v>
+      </c>
+      <c r="J131" t="n">
         <v>8</v>
-      </c>
-      <c r="J131" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -5717,10 +5717,10 @@
         <v>43</v>
       </c>
       <c r="G132" t="n">
+        <v>9</v>
+      </c>
+      <c r="H132" t="n">
         <v>11</v>
-      </c>
-      <c r="H132" t="n">
-        <v>9</v>
       </c>
       <c r="I132" t="n">
         <v>1</v>
@@ -5757,16 +5757,16 @@
         <v>16</v>
       </c>
       <c r="G133" t="n">
+        <v>4</v>
+      </c>
+      <c r="H133" t="n">
         <v>16</v>
       </c>
-      <c r="H133" t="n">
-        <v>4</v>
-      </c>
       <c r="I133" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J133" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -5803,10 +5803,10 @@
         <v>4</v>
       </c>
       <c r="I134" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J134" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135">
@@ -5837,16 +5837,16 @@
         <v>25</v>
       </c>
       <c r="G135" t="n">
+        <v>7</v>
+      </c>
+      <c r="H135" t="n">
         <v>5</v>
       </c>
-      <c r="H135" t="n">
-        <v>7</v>
-      </c>
       <c r="I135" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J135" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
@@ -5877,16 +5877,16 @@
         <v>33</v>
       </c>
       <c r="G136" t="n">
+        <v>5</v>
+      </c>
+      <c r="H136" t="n">
         <v>16</v>
       </c>
-      <c r="H136" t="n">
-        <v>5</v>
-      </c>
       <c r="I136" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J136" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137">
@@ -5923,10 +5923,10 @@
         <v>6</v>
       </c>
       <c r="I137" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J137" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138">
@@ -5957,10 +5957,10 @@
         <v>15</v>
       </c>
       <c r="G138" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H138" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I138" t="n">
         <v>2</v>
@@ -5997,16 +5997,16 @@
         <v>22</v>
       </c>
       <c r="G139" t="n">
+        <v>5</v>
+      </c>
+      <c r="H139" t="n">
         <v>15</v>
       </c>
-      <c r="H139" t="n">
-        <v>5</v>
-      </c>
       <c r="I139" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J139" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140">
@@ -6037,16 +6037,16 @@
         <v>19</v>
       </c>
       <c r="G140" t="n">
+        <v>8</v>
+      </c>
+      <c r="H140" t="n">
         <v>15</v>
       </c>
-      <c r="H140" t="n">
-        <v>8</v>
-      </c>
       <c r="I140" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J140" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -6083,10 +6083,10 @@
         <v>10</v>
       </c>
       <c r="I141" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J141" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -6117,16 +6117,16 @@
         <v>42</v>
       </c>
       <c r="G142" t="n">
+        <v>1</v>
+      </c>
+      <c r="H142" t="n">
         <v>5</v>
       </c>
-      <c r="H142" t="n">
-        <v>1</v>
-      </c>
       <c r="I142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -6157,16 +6157,16 @@
         <v>14</v>
       </c>
       <c r="G143" t="n">
+        <v>10</v>
+      </c>
+      <c r="H143" t="n">
         <v>11</v>
       </c>
-      <c r="H143" t="n">
-        <v>10</v>
-      </c>
       <c r="I143" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J143" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -6197,16 +6197,16 @@
         <v>12</v>
       </c>
       <c r="G144" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H144" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I144" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J144" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145">
@@ -6237,16 +6237,16 @@
         <v>21</v>
       </c>
       <c r="G145" t="n">
+        <v>16</v>
+      </c>
+      <c r="H145" t="n">
         <v>18</v>
       </c>
-      <c r="H145" t="n">
-        <v>16</v>
-      </c>
       <c r="I145" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J145" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
@@ -6277,10 +6277,10 @@
         <v>44</v>
       </c>
       <c r="G146" t="n">
+        <v>10</v>
+      </c>
+      <c r="H146" t="n">
         <v>5</v>
-      </c>
-      <c r="H146" t="n">
-        <v>10</v>
       </c>
       <c r="I146" t="n">
         <v>0</v>
@@ -6317,16 +6317,16 @@
         <v>35</v>
       </c>
       <c r="G147" t="n">
+        <v>5</v>
+      </c>
+      <c r="H147" t="n">
         <v>18</v>
       </c>
-      <c r="H147" t="n">
-        <v>5</v>
-      </c>
       <c r="I147" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J147" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
@@ -6357,16 +6357,16 @@
         <v>52</v>
       </c>
       <c r="G148" t="n">
+        <v>4</v>
+      </c>
+      <c r="H148" t="n">
         <v>6</v>
       </c>
-      <c r="H148" t="n">
-        <v>4</v>
-      </c>
       <c r="I148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -6437,16 +6437,16 @@
         <v>12</v>
       </c>
       <c r="G150" t="n">
+        <v>14</v>
+      </c>
+      <c r="H150" t="n">
         <v>5</v>
       </c>
-      <c r="H150" t="n">
-        <v>14</v>
-      </c>
       <c r="I150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J150" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -6477,16 +6477,16 @@
         <v>31</v>
       </c>
       <c r="G151" t="n">
+        <v>14</v>
+      </c>
+      <c r="H151" t="n">
         <v>8</v>
       </c>
-      <c r="H151" t="n">
-        <v>14</v>
-      </c>
       <c r="I151" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J151" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -6517,16 +6517,16 @@
         <v>8</v>
       </c>
       <c r="G152" t="n">
+        <v>3</v>
+      </c>
+      <c r="H152" t="n">
         <v>5</v>
       </c>
-      <c r="H152" t="n">
-        <v>3</v>
-      </c>
       <c r="I152" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J152" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -6563,10 +6563,10 @@
         <v>8</v>
       </c>
       <c r="I153" t="n">
+        <v>3</v>
+      </c>
+      <c r="J153" t="n">
         <v>6</v>
-      </c>
-      <c r="J153" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="154">
@@ -6597,16 +6597,16 @@
         <v>12</v>
       </c>
       <c r="G154" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I154" t="n">
+        <v>3</v>
+      </c>
+      <c r="J154" t="n">
         <v>5</v>
-      </c>
-      <c r="J154" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="155">
@@ -6637,16 +6637,16 @@
         <v>32</v>
       </c>
       <c r="G155" t="n">
+        <v>0</v>
+      </c>
+      <c r="H155" t="n">
         <v>17</v>
       </c>
-      <c r="H155" t="n">
-        <v>0</v>
-      </c>
       <c r="I155" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J155" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -6677,16 +6677,16 @@
         <v>31</v>
       </c>
       <c r="G156" t="n">
+        <v>10</v>
+      </c>
+      <c r="H156" t="n">
         <v>19</v>
       </c>
-      <c r="H156" t="n">
-        <v>10</v>
-      </c>
       <c r="I156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -6717,16 +6717,16 @@
         <v>16</v>
       </c>
       <c r="G157" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H157" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I157" t="n">
+        <v>1</v>
+      </c>
+      <c r="J157" t="n">
         <v>5</v>
-      </c>
-      <c r="J157" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -6757,16 +6757,16 @@
         <v>16</v>
       </c>
       <c r="G158" t="n">
+        <v>14</v>
+      </c>
+      <c r="H158" t="n">
         <v>12</v>
       </c>
-      <c r="H158" t="n">
-        <v>14</v>
-      </c>
       <c r="I158" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J158" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159">
@@ -6797,16 +6797,16 @@
         <v>5</v>
       </c>
       <c r="G159" t="n">
+        <v>2</v>
+      </c>
+      <c r="H159" t="n">
         <v>19</v>
       </c>
-      <c r="H159" t="n">
-        <v>2</v>
-      </c>
       <c r="I159" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J159" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -6837,16 +6837,16 @@
         <v>21</v>
       </c>
       <c r="G160" t="n">
+        <v>4</v>
+      </c>
+      <c r="H160" t="n">
         <v>16</v>
       </c>
-      <c r="H160" t="n">
-        <v>4</v>
-      </c>
       <c r="I160" t="n">
+        <v>1</v>
+      </c>
+      <c r="J160" t="n">
         <v>3</v>
-      </c>
-      <c r="J160" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -6877,10 +6877,10 @@
         <v>27</v>
       </c>
       <c r="G161" t="n">
+        <v>0</v>
+      </c>
+      <c r="H161" t="n">
         <v>11</v>
-      </c>
-      <c r="H161" t="n">
-        <v>0</v>
       </c>
       <c r="I161" t="n">
         <v>2</v>
@@ -6917,10 +6917,10 @@
         <v>4</v>
       </c>
       <c r="G162" t="n">
+        <v>11</v>
+      </c>
+      <c r="H162" t="n">
         <v>5</v>
-      </c>
-      <c r="H162" t="n">
-        <v>11</v>
       </c>
       <c r="I162" t="n">
         <v>2</v>
@@ -6957,10 +6957,10 @@
         <v>7</v>
       </c>
       <c r="G163" t="n">
+        <v>7</v>
+      </c>
+      <c r="H163" t="n">
         <v>12</v>
-      </c>
-      <c r="H163" t="n">
-        <v>7</v>
       </c>
       <c r="I163" t="n">
         <v>2</v>
@@ -6997,16 +6997,16 @@
         <v>14</v>
       </c>
       <c r="G164" t="n">
+        <v>1</v>
+      </c>
+      <c r="H164" t="n">
         <v>24</v>
       </c>
-      <c r="H164" t="n">
-        <v>1</v>
-      </c>
       <c r="I164" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J164" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -7037,16 +7037,16 @@
         <v>17</v>
       </c>
       <c r="G165" t="n">
+        <v>4</v>
+      </c>
+      <c r="H165" t="n">
         <v>7</v>
       </c>
-      <c r="H165" t="n">
-        <v>4</v>
-      </c>
       <c r="I165" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J165" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
@@ -7077,16 +7077,16 @@
         <v>55</v>
       </c>
       <c r="G166" t="n">
+        <v>7</v>
+      </c>
+      <c r="H166" t="n">
         <v>3</v>
       </c>
-      <c r="H166" t="n">
-        <v>7</v>
-      </c>
       <c r="I166" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -7117,16 +7117,16 @@
         <v>41</v>
       </c>
       <c r="G167" t="n">
+        <v>4</v>
+      </c>
+      <c r="H167" t="n">
         <v>5</v>
       </c>
-      <c r="H167" t="n">
-        <v>4</v>
-      </c>
       <c r="I167" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J167" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="168">
@@ -7157,16 +7157,16 @@
         <v>5</v>
       </c>
       <c r="G168" t="n">
+        <v>12</v>
+      </c>
+      <c r="H168" t="n">
         <v>5</v>
       </c>
-      <c r="H168" t="n">
-        <v>12</v>
-      </c>
       <c r="I168" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J168" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -7203,10 +7203,10 @@
         <v>2</v>
       </c>
       <c r="I169" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J169" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -7237,10 +7237,10 @@
         <v>23</v>
       </c>
       <c r="G170" t="n">
+        <v>7</v>
+      </c>
+      <c r="H170" t="n">
         <v>3</v>
-      </c>
-      <c r="H170" t="n">
-        <v>7</v>
       </c>
       <c r="I170" t="n">
         <v>2</v>
@@ -7277,10 +7277,10 @@
         <v>54</v>
       </c>
       <c r="G171" t="n">
+        <v>9</v>
+      </c>
+      <c r="H171" t="n">
         <v>5</v>
-      </c>
-      <c r="H171" t="n">
-        <v>9</v>
       </c>
       <c r="I171" t="n">
         <v>3</v>
@@ -7317,16 +7317,16 @@
         <v>17</v>
       </c>
       <c r="G172" t="n">
+        <v>4</v>
+      </c>
+      <c r="H172" t="n">
         <v>21</v>
       </c>
-      <c r="H172" t="n">
-        <v>4</v>
-      </c>
       <c r="I172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J172" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -7357,16 +7357,16 @@
         <v>23</v>
       </c>
       <c r="G173" t="n">
+        <v>4</v>
+      </c>
+      <c r="H173" t="n">
         <v>3</v>
       </c>
-      <c r="H173" t="n">
-        <v>4</v>
-      </c>
       <c r="I173" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J173" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174">
@@ -7397,16 +7397,16 @@
         <v>30</v>
       </c>
       <c r="G174" t="n">
+        <v>8</v>
+      </c>
+      <c r="H174" t="n">
         <v>12</v>
       </c>
-      <c r="H174" t="n">
-        <v>8</v>
-      </c>
       <c r="I174" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J174" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -7437,10 +7437,10 @@
         <v>47</v>
       </c>
       <c r="G175" t="n">
+        <v>2</v>
+      </c>
+      <c r="H175" t="n">
         <v>7</v>
-      </c>
-      <c r="H175" t="n">
-        <v>2</v>
       </c>
       <c r="I175" t="n">
         <v>2</v>
@@ -7517,16 +7517,16 @@
         <v>33</v>
       </c>
       <c r="G177" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H177" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I177" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J177" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178">
@@ -7557,16 +7557,16 @@
         <v>26</v>
       </c>
       <c r="G178" t="n">
+        <v>6</v>
+      </c>
+      <c r="H178" t="n">
         <v>8</v>
       </c>
-      <c r="H178" t="n">
-        <v>6</v>
-      </c>
       <c r="I178" t="n">
+        <v>2</v>
+      </c>
+      <c r="J178" t="n">
         <v>3</v>
-      </c>
-      <c r="J178" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="179">
@@ -7597,10 +7597,10 @@
         <v>25</v>
       </c>
       <c r="G179" t="n">
+        <v>9</v>
+      </c>
+      <c r="H179" t="n">
         <v>10</v>
-      </c>
-      <c r="H179" t="n">
-        <v>9</v>
       </c>
       <c r="I179" t="n">
         <v>3</v>
@@ -7643,10 +7643,10 @@
         <v>5</v>
       </c>
       <c r="I180" t="n">
+        <v>2</v>
+      </c>
+      <c r="J180" t="n">
         <v>7</v>
-      </c>
-      <c r="J180" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="181">
@@ -7677,16 +7677,16 @@
         <v>19</v>
       </c>
       <c r="G181" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H181" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I181" t="n">
+        <v>0</v>
+      </c>
+      <c r="J181" t="n">
         <v>7</v>
-      </c>
-      <c r="J181" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -7717,16 +7717,16 @@
         <v>41</v>
       </c>
       <c r="G182" t="n">
+        <v>11</v>
+      </c>
+      <c r="H182" t="n">
         <v>14</v>
       </c>
-      <c r="H182" t="n">
-        <v>11</v>
-      </c>
       <c r="I182" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J182" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -7757,16 +7757,16 @@
         <v>28</v>
       </c>
       <c r="G183" t="n">
+        <v>8</v>
+      </c>
+      <c r="H183" t="n">
         <v>10</v>
       </c>
-      <c r="H183" t="n">
-        <v>8</v>
-      </c>
       <c r="I183" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J183" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">
@@ -7797,16 +7797,16 @@
         <v>31</v>
       </c>
       <c r="G184" t="n">
+        <v>14</v>
+      </c>
+      <c r="H184" t="n">
         <v>18</v>
       </c>
-      <c r="H184" t="n">
-        <v>14</v>
-      </c>
       <c r="I184" t="n">
+        <v>0</v>
+      </c>
+      <c r="J184" t="n">
         <v>7</v>
-      </c>
-      <c r="J184" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -7837,16 +7837,16 @@
         <v>32</v>
       </c>
       <c r="G185" t="n">
+        <v>2</v>
+      </c>
+      <c r="H185" t="n">
         <v>11</v>
       </c>
-      <c r="H185" t="n">
-        <v>2</v>
-      </c>
       <c r="I185" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J185" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186">
@@ -7877,16 +7877,16 @@
         <v>28</v>
       </c>
       <c r="G186" t="n">
+        <v>6</v>
+      </c>
+      <c r="H186" t="n">
         <v>13</v>
       </c>
-      <c r="H186" t="n">
-        <v>6</v>
-      </c>
       <c r="I186" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J186" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="187">
@@ -7917,16 +7917,16 @@
         <v>19</v>
       </c>
       <c r="G187" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H187" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I187" t="n">
+        <v>4</v>
+      </c>
+      <c r="J187" t="n">
         <v>3</v>
-      </c>
-      <c r="J187" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="188">
@@ -7957,16 +7957,16 @@
         <v>18</v>
       </c>
       <c r="G188" t="n">
+        <v>7</v>
+      </c>
+      <c r="H188" t="n">
         <v>5</v>
       </c>
-      <c r="H188" t="n">
-        <v>7</v>
-      </c>
       <c r="I188" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J188" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -7997,16 +7997,16 @@
         <v>13</v>
       </c>
       <c r="G189" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H189" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I189" t="n">
+        <v>0</v>
+      </c>
+      <c r="J189" t="n">
         <v>7</v>
-      </c>
-      <c r="J189" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="190">
@@ -8037,16 +8037,16 @@
         <v>38</v>
       </c>
       <c r="G190" t="n">
+        <v>5</v>
+      </c>
+      <c r="H190" t="n">
         <v>12</v>
       </c>
-      <c r="H190" t="n">
+      <c r="I190" t="n">
         <v>5</v>
       </c>
-      <c r="I190" t="n">
-        <v>1</v>
-      </c>
       <c r="J190" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -8077,16 +8077,16 @@
         <v>13</v>
       </c>
       <c r="G191" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H191" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I191" t="n">
+        <v>0</v>
+      </c>
+      <c r="J191" t="n">
         <v>7</v>
-      </c>
-      <c r="J191" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -8117,16 +8117,16 @@
         <v>46</v>
       </c>
       <c r="G192" t="n">
+        <v>11</v>
+      </c>
+      <c r="H192" t="n">
         <v>12</v>
       </c>
-      <c r="H192" t="n">
-        <v>11</v>
-      </c>
       <c r="I192" t="n">
+        <v>2</v>
+      </c>
+      <c r="J192" t="n">
         <v>5</v>
-      </c>
-      <c r="J192" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="193">
@@ -8157,10 +8157,10 @@
         <v>21</v>
       </c>
       <c r="G193" t="n">
+        <v>1</v>
+      </c>
+      <c r="H193" t="n">
         <v>16</v>
-      </c>
-      <c r="H193" t="n">
-        <v>1</v>
       </c>
       <c r="I193" t="n">
         <v>2</v>
@@ -8197,16 +8197,16 @@
         <v>16</v>
       </c>
       <c r="G194" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H194" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I194" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J194" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195">
@@ -8237,16 +8237,16 @@
         <v>18</v>
       </c>
       <c r="G195" t="n">
+        <v>13</v>
+      </c>
+      <c r="H195" t="n">
         <v>9</v>
       </c>
-      <c r="H195" t="n">
-        <v>13</v>
-      </c>
       <c r="I195" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J195" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196">
@@ -8277,16 +8277,16 @@
         <v>25</v>
       </c>
       <c r="G196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I196" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J196" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="197">
@@ -8317,10 +8317,10 @@
         <v>13</v>
       </c>
       <c r="G197" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H197" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I197" t="n">
         <v>0</v>
@@ -8357,10 +8357,10 @@
         <v>41</v>
       </c>
       <c r="G198" t="n">
+        <v>9</v>
+      </c>
+      <c r="H198" t="n">
         <v>15</v>
-      </c>
-      <c r="H198" t="n">
-        <v>9</v>
       </c>
       <c r="I198" t="n">
         <v>2</v>
@@ -8397,16 +8397,16 @@
         <v>33</v>
       </c>
       <c r="G199" t="n">
+        <v>3</v>
+      </c>
+      <c r="H199" t="n">
         <v>19</v>
       </c>
-      <c r="H199" t="n">
+      <c r="I199" t="n">
         <v>3</v>
       </c>
-      <c r="I199" t="n">
-        <v>1</v>
-      </c>
       <c r="J199" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -8443,10 +8443,10 @@
         <v>3</v>
       </c>
       <c r="I200" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J200" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201">
@@ -8477,16 +8477,16 @@
         <v>13</v>
       </c>
       <c r="G201" t="n">
+        <v>0</v>
+      </c>
+      <c r="H201" t="n">
         <v>13</v>
       </c>
-      <c r="H201" t="n">
-        <v>0</v>
-      </c>
       <c r="I201" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J201" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="202">
@@ -8517,10 +8517,10 @@
         <v>20</v>
       </c>
       <c r="G202" t="n">
+        <v>7</v>
+      </c>
+      <c r="H202" t="n">
         <v>16</v>
-      </c>
-      <c r="H202" t="n">
-        <v>7</v>
       </c>
       <c r="I202" t="n">
         <v>1</v>
@@ -8557,16 +8557,16 @@
         <v>22</v>
       </c>
       <c r="G203" t="n">
+        <v>3</v>
+      </c>
+      <c r="H203" t="n">
         <v>22</v>
       </c>
-      <c r="H203" t="n">
-        <v>3</v>
-      </c>
       <c r="I203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204">
@@ -8597,16 +8597,16 @@
         <v>30</v>
       </c>
       <c r="G204" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H204" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I204" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J204" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205">
@@ -8637,16 +8637,16 @@
         <v>23</v>
       </c>
       <c r="G205" t="n">
+        <v>6</v>
+      </c>
+      <c r="H205" t="n">
         <v>3</v>
       </c>
-      <c r="H205" t="n">
-        <v>6</v>
-      </c>
       <c r="I205" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J205" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206">
@@ -8683,10 +8683,10 @@
         <v>4</v>
       </c>
       <c r="I206" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J206" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207">
@@ -8717,16 +8717,16 @@
         <v>26</v>
       </c>
       <c r="G207" t="n">
+        <v>6</v>
+      </c>
+      <c r="H207" t="n">
         <v>12</v>
       </c>
-      <c r="H207" t="n">
-        <v>6</v>
-      </c>
       <c r="I207" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J207" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208">
@@ -8757,16 +8757,16 @@
         <v>9</v>
       </c>
       <c r="G208" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H208" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I208" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J208" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="209">
@@ -8797,10 +8797,10 @@
         <v>2</v>
       </c>
       <c r="G209" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H209" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I209" t="n">
         <v>4</v>
@@ -8837,16 +8837,16 @@
         <v>28</v>
       </c>
       <c r="G210" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H210" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
@@ -8883,10 +8883,10 @@
         <v>5</v>
       </c>
       <c r="I211" t="n">
+        <v>0</v>
+      </c>
+      <c r="J211" t="n">
         <v>6</v>
-      </c>
-      <c r="J211" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -8917,10 +8917,10 @@
         <v>26</v>
       </c>
       <c r="G212" t="n">
+        <v>14</v>
+      </c>
+      <c r="H212" t="n">
         <v>8</v>
-      </c>
-      <c r="H212" t="n">
-        <v>14</v>
       </c>
       <c r="I212" t="n">
         <v>2</v>
@@ -8957,16 +8957,16 @@
         <v>27</v>
       </c>
       <c r="G213" t="n">
+        <v>6</v>
+      </c>
+      <c r="H213" t="n">
         <v>18</v>
       </c>
-      <c r="H213" t="n">
-        <v>6</v>
-      </c>
       <c r="I213" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J213" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214">
@@ -8997,16 +8997,16 @@
         <v>20</v>
       </c>
       <c r="G214" t="n">
+        <v>1</v>
+      </c>
+      <c r="H214" t="n">
         <v>12</v>
       </c>
-      <c r="H214" t="n">
-        <v>1</v>
-      </c>
       <c r="I214" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J214" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="215">
@@ -9037,16 +9037,16 @@
         <v>28</v>
       </c>
       <c r="G215" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="H215" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I215" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J215" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="216">
@@ -9083,10 +9083,10 @@
         <v>2</v>
       </c>
       <c r="I216" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J216" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -9117,16 +9117,16 @@
         <v>25</v>
       </c>
       <c r="G217" t="n">
+        <v>1</v>
+      </c>
+      <c r="H217" t="n">
         <v>3</v>
       </c>
-      <c r="H217" t="n">
-        <v>1</v>
-      </c>
       <c r="I217" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J217" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218">
@@ -9157,10 +9157,10 @@
         <v>51</v>
       </c>
       <c r="G218" t="n">
+        <v>3</v>
+      </c>
+      <c r="H218" t="n">
         <v>14</v>
-      </c>
-      <c r="H218" t="n">
-        <v>3</v>
       </c>
       <c r="I218" t="n">
         <v>0</v>
@@ -9197,10 +9197,10 @@
         <v>40</v>
       </c>
       <c r="G219" t="n">
+        <v>9</v>
+      </c>
+      <c r="H219" t="n">
         <v>14</v>
-      </c>
-      <c r="H219" t="n">
-        <v>9</v>
       </c>
       <c r="I219" t="n">
         <v>2</v>
@@ -9237,10 +9237,10 @@
         <v>41</v>
       </c>
       <c r="G220" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H220" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I220" t="n">
         <v>0</v>
@@ -9277,16 +9277,16 @@
         <v>31</v>
       </c>
       <c r="G221" t="n">
+        <v>4</v>
+      </c>
+      <c r="H221" t="n">
         <v>14</v>
       </c>
-      <c r="H221" t="n">
-        <v>4</v>
-      </c>
       <c r="I221" t="n">
+        <v>6</v>
+      </c>
+      <c r="J221" t="n">
         <v>3</v>
-      </c>
-      <c r="J221" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="222">
@@ -9317,16 +9317,16 @@
         <v>4</v>
       </c>
       <c r="G222" t="n">
+        <v>3</v>
+      </c>
+      <c r="H222" t="n">
         <v>6</v>
       </c>
-      <c r="H222" t="n">
+      <c r="I222" t="n">
         <v>3</v>
       </c>
-      <c r="I222" t="n">
-        <v>2</v>
-      </c>
       <c r="J222" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="223">
@@ -9357,16 +9357,16 @@
         <v>51</v>
       </c>
       <c r="G223" t="n">
+        <v>9</v>
+      </c>
+      <c r="H223" t="n">
         <v>11</v>
       </c>
-      <c r="H223" t="n">
-        <v>9</v>
-      </c>
       <c r="I223" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J223" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224">
@@ -9397,16 +9397,16 @@
         <v>31</v>
       </c>
       <c r="G224" t="n">
+        <v>1</v>
+      </c>
+      <c r="H224" t="n">
         <v>11</v>
       </c>
-      <c r="H224" t="n">
-        <v>1</v>
-      </c>
       <c r="I224" t="n">
+        <v>1</v>
+      </c>
+      <c r="J224" t="n">
         <v>3</v>
-      </c>
-      <c r="J224" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="225">
@@ -9437,16 +9437,16 @@
         <v>31</v>
       </c>
       <c r="G225" t="n">
+        <v>7</v>
+      </c>
+      <c r="H225" t="n">
         <v>20</v>
       </c>
-      <c r="H225" t="n">
-        <v>7</v>
-      </c>
       <c r="I225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226">
@@ -9477,16 +9477,16 @@
         <v>29</v>
       </c>
       <c r="G226" t="n">
+        <v>2</v>
+      </c>
+      <c r="H226" t="n">
         <v>11</v>
       </c>
-      <c r="H226" t="n">
-        <v>2</v>
-      </c>
       <c r="I226" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J226" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227">
@@ -9517,16 +9517,16 @@
         <v>55</v>
       </c>
       <c r="G227" t="n">
+        <v>5</v>
+      </c>
+      <c r="H227" t="n">
         <v>8</v>
       </c>
-      <c r="H227" t="n">
-        <v>5</v>
-      </c>
       <c r="I227" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J227" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="228">
@@ -9557,16 +9557,16 @@
         <v>40</v>
       </c>
       <c r="G228" t="n">
+        <v>1</v>
+      </c>
+      <c r="H228" t="n">
         <v>15</v>
       </c>
-      <c r="H228" t="n">
-        <v>1</v>
-      </c>
       <c r="I228" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J228" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -9597,16 +9597,16 @@
         <v>4</v>
       </c>
       <c r="G229" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H229" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I229" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J229" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="230">
@@ -9637,16 +9637,16 @@
         <v>8</v>
       </c>
       <c r="G230" t="n">
+        <v>9</v>
+      </c>
+      <c r="H230" t="n">
         <v>7</v>
       </c>
-      <c r="H230" t="n">
-        <v>9</v>
-      </c>
       <c r="I230" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J230" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>